<commit_message>
Forgot I2C pullup resistors, updated Sch, PCB, and BOM
</commit_message>
<xml_diff>
--- a/docs/BOM.xlsx
+++ b/docs/BOM.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\DATA\Projects\pico-vga\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F069ADD-8B6D-4E77-82E6-B5A1EED384D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8847281D-C444-473F-9E5D-F2863FF23E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{135CBA0D-5FA5-414C-B0B9-8FCA77DD5795}"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM_Custom" sheetId="3" r:id="rId1"/>
+    <sheet name="BOM_Custom" sheetId="5" r:id="rId1"/>
     <sheet name="BOM" sheetId="2" r:id="rId2"/>
     <sheet name="BOM_Export" sheetId="1" r:id="rId3"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="204">
   <si>
     <t>Item</t>
   </si>
@@ -130,21 +130,6 @@
     <t>J2</t>
   </si>
   <si>
-    <t>Micro_SD_Card</t>
-  </si>
-  <si>
-    <t>Connector:Micro_SD_Card</t>
-  </si>
-  <si>
-    <t>Connector_Card:microSD_HC_Hirose_DM3AT-SF-PEJM5</t>
-  </si>
-  <si>
-    <t>http://katalog.we-online.de/em/datasheet/693072010801.pdf</t>
-  </si>
-  <si>
-    <t>DM3AT-SF-PEJM5</t>
-  </si>
-  <si>
     <t>J3, J4, J8, J9</t>
   </si>
   <si>
@@ -181,12 +166,6 @@
     <t>Connector:AudioJack3</t>
   </si>
   <si>
-    <t>Connector_Audio:Jack_3.5mm_CUI_SJ1-3533NG_Horizontal</t>
-  </si>
-  <si>
-    <t>SJ1-3533NG</t>
-  </si>
-  <si>
     <t>J7</t>
   </si>
   <si>
@@ -211,9 +190,6 @@
     <t>Package_TO_SOT_SMD:SOT-23</t>
   </si>
   <si>
-    <t>R1, R12</t>
-  </si>
-  <si>
     <t>1K</t>
   </si>
   <si>
@@ -241,24 +217,9 @@
     <t>2.2K</t>
   </si>
   <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>R13, R17, R18, R22, R23</t>
-  </si>
-  <si>
     <t>1M</t>
   </si>
   <si>
-    <t>R14, R19</t>
-  </si>
-  <si>
-    <t>R15, R20</t>
-  </si>
-  <si>
     <t>R16, R21</t>
   </si>
   <si>
@@ -322,15 +283,9 @@
     <t>Total Cost</t>
   </si>
   <si>
-    <t>47uF 0805 Cap</t>
-  </si>
-  <si>
     <t xml:space="preserve">pico-vga </t>
   </si>
   <si>
-    <t>100nF 0805 Cap</t>
-  </si>
-  <si>
     <t>Blue LED 0805</t>
   </si>
   <si>
@@ -358,39 +313,6 @@
     <t>PMOS 30V 3.8A</t>
   </si>
   <si>
-    <t>1k 0805 Res</t>
-  </si>
-  <si>
-    <t>470R 0805 Res</t>
-  </si>
-  <si>
-    <t>33R 0805 Res</t>
-  </si>
-  <si>
-    <t>1.2k 0805 Res</t>
-  </si>
-  <si>
-    <t>2.2k 0805 Res</t>
-  </si>
-  <si>
-    <t>390R 0805 Res</t>
-  </si>
-  <si>
-    <t>47R 0805 Res</t>
-  </si>
-  <si>
-    <t>1M 0805 Res</t>
-  </si>
-  <si>
-    <t>220R 0805 Res</t>
-  </si>
-  <si>
-    <t>100R 0805 Res</t>
-  </si>
-  <si>
-    <t>1.8k 0805 Res</t>
-  </si>
-  <si>
     <t>Reset Button</t>
   </si>
   <si>
@@ -638,6 +560,96 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21B104KBCNNNC/3886661</t>
+  </si>
+  <si>
+    <t>Micro_SD_Card_Det</t>
+  </si>
+  <si>
+    <t>Connector:Micro_SD_Card_Det</t>
+  </si>
+  <si>
+    <t>pico-vga:MEM2061-01-188-00-A_GCT</t>
+  </si>
+  <si>
+    <t>https://www.hirose.com/product/en/download_file/key_name/DM3/category/Catalog/doc_file_id/49662/?file_category_id=4&amp;item_id=195&amp;is_series=1</t>
+  </si>
+  <si>
+    <t>pico-vga:STX-3000_KYC</t>
+  </si>
+  <si>
+    <t>R1, R14</t>
+  </si>
+  <si>
+    <t>R10, R11</t>
+  </si>
+  <si>
+    <t>4.7k</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R15, R19, R20, R24, R25</t>
+  </si>
+  <si>
+    <t>R17, R22</t>
+  </si>
+  <si>
+    <t>R18, R23</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF4701V</t>
+  </si>
+  <si>
+    <t>P4.70KCCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-6ENF4701V/954352?s=N4IgjCBcoExaBjKAzAhgGwM4FMA0IB7KAbXAAYAOAdgE4QBdfABwBcoQBlFgJwEsA7AOYgAvvgDM8EEkhoseQiXBhxERiFbsufIaPxgAbFJlyc%2BIpFLia4mHXWbInHgOFjwNCnWjSUGM4qWIGQM7jCUAKzGfvLmSgAsAHRUAAQA1gDyABYAtpgMzGxOAKr8vCwZyACy2KiYAK7c2HogALRwPjI89QoWpFH07q1GnVDdvUqSg-it3ohj3D1xQWpDEKOy-hMrIYNhSk2YvJgsBNyhQA</t>
+  </si>
+  <si>
+    <t>47uF 0805 Cap (5V or more)</t>
+  </si>
+  <si>
+    <t>100nF 0805 Cap (5V or more)</t>
+  </si>
+  <si>
+    <t>1k 0805 Res 1%</t>
+  </si>
+  <si>
+    <t>470R 0805 Res 1%</t>
+  </si>
+  <si>
+    <t>33R 0805 Res 1%</t>
+  </si>
+  <si>
+    <t>1.2k 0805 Res 1%</t>
+  </si>
+  <si>
+    <t>2.2k 0805 Res 1%</t>
+  </si>
+  <si>
+    <t>4.7k 0805 Res 1%</t>
+  </si>
+  <si>
+    <t>390R 0805 Res 1%</t>
+  </si>
+  <si>
+    <t>47R 0805 Res 1%</t>
+  </si>
+  <si>
+    <t>1M 0805 Res 1%</t>
+  </si>
+  <si>
+    <t>220R 0805 Res 1%</t>
+  </si>
+  <si>
+    <t>100R 0805 Res 1%</t>
+  </si>
+  <si>
+    <t>1.8k 0805 Res 1%</t>
   </si>
 </sst>
 </file>
@@ -722,10 +734,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1024,8 +1032,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41676850-015E-4523-B008-90A3DF7CB11C}">
-  <dimension ref="A1:N51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCE2567-DB3F-4561-9ED3-12DD0FC8DD03}">
+  <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1050,48 +1058,48 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="J1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="M1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="N1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>190</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1101,19 +1109,19 @@
         <v>pico-vga C1, C3, C5</v>
       </c>
       <c r="D2" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="E2" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="I2" s="1">
         <v>0.28999999999999998</v>
@@ -1126,38 +1134,38 @@
         <v>0.86999999999999988</v>
       </c>
       <c r="M2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="N2" s="1">
         <f>SUM(K:K)</f>
-        <v>13.639999999999997</v>
+        <v>13.839999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C25" si="0">_xlfn.CONCAT($N$1, B3)</f>
+        <f t="shared" ref="C3:C26" si="0">_xlfn.CONCAT($N$1, B3)</f>
         <v>pico-vga C2, C4</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="E3" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="I3" s="1">
         <v>0.1</v>
@@ -1166,13 +1174,13 @@
         <v>2</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K51" si="1">I3*J3</f>
+        <f t="shared" ref="K3:K52" si="1">I3*J3</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -1182,16 +1190,16 @@
         <v>pico-vga D1</v>
       </c>
       <c r="D4" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="E4" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="I4" s="1">
         <v>0.19</v>
@@ -1206,7 +1214,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -1219,13 +1227,13 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="I5" s="1">
         <v>0.21</v>
@@ -1240,7 +1248,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
@@ -1253,13 +1261,13 @@
         <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="I6" s="1">
         <v>1.46</v>
@@ -1274,7 +1282,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
@@ -1284,16 +1292,16 @@
         <v>pico-vga J2</v>
       </c>
       <c r="D7" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="E7" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="I7" s="1">
         <v>1.2</v>
@@ -1308,26 +1316,26 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga J3, J4, J8, J9</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="I8" s="1">
         <v>0.48</v>
@@ -1342,17 +1350,17 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga J5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -1364,26 +1372,26 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga J6</v>
       </c>
       <c r="D10" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="E10" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="I10" s="1">
         <v>0.8</v>
@@ -1398,17 +1406,17 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga J7</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1420,26 +1428,26 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga Q1</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="I12" s="1">
         <v>0.34</v>
@@ -1454,29 +1462,29 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>192</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R1, R12</v>
+        <v>pico-vga R1, R14</v>
       </c>
       <c r="D13" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="E13" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="I13" s="1">
         <v>0.1</v>
@@ -1491,29 +1499,29 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>107</v>
+        <v>193</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga R2, R6</v>
       </c>
       <c r="D14" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="E14" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="I14" s="1">
         <v>0.1</v>
@@ -1528,29 +1536,29 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>194</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga R3, R7</v>
       </c>
       <c r="D15" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="E15" t="s">
-        <v>180</v>
+        <v>154</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="I15" s="1">
         <v>0.1</v>
@@ -1565,29 +1573,29 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>109</v>
+        <v>195</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga R4, R8</v>
       </c>
       <c r="D16" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="E16" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="I16" s="1">
         <v>0.1</v>
@@ -1602,29 +1610,29 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>196</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga R5, R9</v>
       </c>
       <c r="D17" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="E17" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="I17" s="1">
         <v>0.1</v>
@@ -1639,66 +1647,66 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>197</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>180</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R10</v>
+        <v>pico-vga R10, R11</v>
       </c>
       <c r="D18" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="E18" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>133</v>
+        <v>181</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="I18" s="1">
         <v>0.1</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K18" s="1">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>198</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>182</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R11</v>
+        <v>pico-vga R12</v>
       </c>
       <c r="D19" t="s">
-        <v>191</v>
+        <v>150</v>
       </c>
       <c r="E19" t="s">
-        <v>192</v>
+        <v>151</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>193</v>
+        <v>152</v>
       </c>
       <c r="I19" s="1">
         <v>0.1</v>
@@ -1713,103 +1721,103 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>199</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>183</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R13, R17, R18, R22, R23</v>
+        <v>pico-vga R13</v>
       </c>
       <c r="D20" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="E20" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="I20" s="1">
         <v>0.1</v>
       </c>
       <c r="J20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K20" s="1">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>200</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R14, R19</v>
+        <v>pico-vga R15, R19, R20, R24, R25</v>
       </c>
       <c r="D21" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="E21" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>135</v>
+        <v>59</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="I21" s="1">
         <v>0.1</v>
       </c>
       <c r="J21">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K21" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>201</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R15, R20</v>
+        <v>pico-vga R16, R21</v>
       </c>
       <c r="D22" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="E22" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="I22" s="1">
         <v>0.1</v>
@@ -1824,29 +1832,29 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>202</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>185</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R16, R21</v>
+        <v>pico-vga R17, R22</v>
       </c>
       <c r="D23" t="s">
-        <v>188</v>
+        <v>141</v>
       </c>
       <c r="E23" t="s">
-        <v>189</v>
+        <v>142</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>190</v>
+        <v>143</v>
       </c>
       <c r="I23" s="1">
         <v>0.1</v>
@@ -1861,76 +1869,107 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>117</v>
+        <v>203</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>186</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga SW1</v>
+        <v>pico-vga R18, R23</v>
       </c>
       <c r="D24" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="E24" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>124</v>
+        <v>93</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="I24" s="1">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="J24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K24" s="1">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga U1</v>
+        <v>pico-vga SW1</v>
       </c>
       <c r="D25" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="E25" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="I25" s="1">
-        <v>4</v>
+        <v>0.15</v>
       </c>
       <c r="J25">
         <v>1</v>
       </c>
       <c r="K25" s="1">
         <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>pico-vga U1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I26" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J26">
+        <v>1</v>
+      </c>
       <c r="K26" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -2083,30 +2122,36 @@
         <v>0</v>
       </c>
     </row>
+    <row r="52" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K52" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{C3943670-D334-4FAC-881A-C084D9B4E51D}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{8453B33C-E27C-4A6E-9F24-76167FFE0D5A}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{1F45F393-7E29-4563-A41D-32FCA93B4E9E}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{E8AB2F55-D124-4C88-BE93-7754876E1F99}"/>
-    <hyperlink ref="H6" r:id="rId5" xr:uid="{86E8A67A-7938-4329-AE54-7FA7B8E27164}"/>
-    <hyperlink ref="H7" r:id="rId6" xr:uid="{F6F87F88-AF48-4CFC-BE3F-215EA6808536}"/>
-    <hyperlink ref="H8" r:id="rId7" xr:uid="{5C139857-F57C-47E5-A665-B00AE15616F8}"/>
-    <hyperlink ref="H10" r:id="rId8" xr:uid="{F6887023-ECBA-4F1A-879C-0915165C147A}"/>
-    <hyperlink ref="H12" r:id="rId9" xr:uid="{E23B089E-DC5A-446B-A089-3D0D291CB77B}"/>
-    <hyperlink ref="H13" r:id="rId10" display="https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-6ENF1001V/111281?s=N4IgjCBcoExaBjKAzAhgGwM4FMA0IB7KAbXAAYAOAdgE4QBdfABwBcoQBlFgJwEsA7AOYgAvvgDM8EEkhoseQiXBhxERiFbsufIaPxgAbFJlyc%2BIpFLia4mHXWbInHgOFjwNCnWjSUGM4qWIGQM7jCUAKzGfvLmSmAABADWAPIAFgC2mAzMbE4Aqvy8LCnIALLYqJgArtzYeiAAtHA%2BMjzVChakUfTujUatUO2dSpK9%2BI3eiEPcHXFBan0Qg7L%2BIwshvWFKdZi8mCwE3KFAA" xr:uid="{A88E5C24-E592-4AC2-8381-4ACA653CD105}"/>
-    <hyperlink ref="H14" r:id="rId11" display="https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-6ENF4700V/1746508?s=N4IgjCBcoExaBjKAzAhgGwM4FMA0IB7KAbXAAYAOAdgE4QBdfABwBcoQBlFgJwEsA7AOYgAvvgDM8EEkhoseQiXBhxERiFbsufIaPxgAbFJlyc%2BIpFLia4mHXWbInHgOFjwNCnWjSUGM4qWIGQM7jCUAKzGfvLmSgAsVGQABADyABYAtpgMzGxOAKr8vCypyACy2KiYAK7c2HogALRwPjI8NQoWpFH07k1GbVAdXUqSffhN3ojD3J1xQWr9EEOy-qOLIX1hSvWYvJgsBNyhQA" xr:uid="{20CAD594-E534-4122-9C9E-5CBB98259CB8}"/>
-    <hyperlink ref="H15" r:id="rId12" xr:uid="{D9C0AA91-F664-471A-83D0-99DC5DE48B04}"/>
-    <hyperlink ref="H16" r:id="rId13" xr:uid="{23053BEB-EE99-4ABB-B9B0-7CED281F5C88}"/>
-    <hyperlink ref="H17" r:id="rId14" xr:uid="{E34D31C8-B691-48B5-894A-976DD7FA5A9A}"/>
-    <hyperlink ref="H18" r:id="rId15" xr:uid="{DC30CFD1-5C16-4F7A-B6B2-7B063165F47C}"/>
-    <hyperlink ref="H19" r:id="rId16" xr:uid="{64D4C0A7-868D-4DF8-AA3D-CE0709999D55}"/>
-    <hyperlink ref="H20" r:id="rId17" xr:uid="{829A5152-1413-4ED1-AD65-2ACE37C987CE}"/>
-    <hyperlink ref="H21" r:id="rId18" xr:uid="{DDB86A52-C5B3-46D5-8ABC-099C6554353C}"/>
-    <hyperlink ref="H22" r:id="rId19" xr:uid="{6FCAB29C-A9A8-445E-965A-3B77996ACB2B}"/>
-    <hyperlink ref="H23" r:id="rId20" xr:uid="{3971B7D7-1F62-4C22-8071-CF13C66BFDEA}"/>
-    <hyperlink ref="H24" r:id="rId21" xr:uid="{A8E5EF7B-3BB3-4864-B86C-B008FB819D0A}"/>
-    <hyperlink ref="H25" r:id="rId22" xr:uid="{53CB6B44-1923-4935-BF28-705CDC91EF58}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{C47512F7-0DAA-4BE6-BFA1-26DEE74CB3CA}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{BC6569AC-BC35-4D24-904A-6ABDA5EDC7CE}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{8776341B-3204-4BB0-8D0E-0F3D826EEAA5}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{7C44B87C-08D8-4941-90D3-24044D980DCC}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{1C21CAEB-46F7-4AFB-97D8-FDE88EE1E357}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{7B497EAA-CA7E-4F20-9B1B-CB46AF8EF7AA}"/>
+    <hyperlink ref="H8" r:id="rId7" xr:uid="{BED54906-8ACB-4F14-83C2-2222E2F1601F}"/>
+    <hyperlink ref="H10" r:id="rId8" xr:uid="{61F094BB-133C-4849-AA5E-A64E986F6577}"/>
+    <hyperlink ref="H12" r:id="rId9" xr:uid="{5874167A-891D-4902-910D-BEB10AC847DA}"/>
+    <hyperlink ref="H13" r:id="rId10" display="https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-6ENF1001V/111281?s=N4IgjCBcoExaBjKAzAhgGwM4FMA0IB7KAbXAAYAOAdgE4QBdfABwBcoQBlFgJwEsA7AOYgAvvgDM8EEkhoseQiXBhxERiFbsufIaPxgAbFJlyc%2BIpFLia4mHXWbInHgOFjwNCnWjSUGM4qWIGQM7jCUAKzGfvLmSmAABADWAPIAFgC2mAzMbE4Aqvy8LCnIALLYqJgArtzYeiAAtHA%2BMjzVChakUfTujUatUO2dSpK9%2BI3eiEPcHXFBan0Qg7L%2BIwshvWFKdZi8mCwE3KFAA" xr:uid="{843498AC-23AF-4C7C-8E69-6933C2F6B689}"/>
+    <hyperlink ref="H14" r:id="rId11" display="https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-6ENF4700V/1746508?s=N4IgjCBcoExaBjKAzAhgGwM4FMA0IB7KAbXAAYAOAdgE4QBdfABwBcoQBlFgJwEsA7AOYgAvvgDM8EEkhoseQiXBhxERiFbsufIaPxgAbFJlyc%2BIpFLia4mHXWbInHgOFjwNCnWjSUGM4qWIGQM7jCUAKzGfvLmSgAsVGQABADyABYAtpgMzGxOAKr8vCypyACy2KiYAK7c2HogALRwPjI8NQoWpFH07k1GbVAdXUqSffhN3ojD3J1xQWr9EEOy-qOLIX1hSvWYvJgsBNyhQA" xr:uid="{FDC50D01-9324-4EBE-9031-1BB648303976}"/>
+    <hyperlink ref="H15" r:id="rId12" xr:uid="{71D2F41C-2893-424A-9F76-A0C70CEA3650}"/>
+    <hyperlink ref="H16" r:id="rId13" xr:uid="{83E26751-A6AF-41B3-8035-689D68DBBED3}"/>
+    <hyperlink ref="H17" r:id="rId14" xr:uid="{97E5C901-985C-41ED-80E5-9AA69D90C7B2}"/>
+    <hyperlink ref="H19" r:id="rId15" xr:uid="{EC43C74C-3F6A-41D7-9417-ACA2B8768492}"/>
+    <hyperlink ref="H20" r:id="rId16" xr:uid="{31CAC340-61BC-4528-9984-0AE84D3560AF}"/>
+    <hyperlink ref="H21" r:id="rId17" xr:uid="{6C616E04-52D4-42F5-BA64-8BACA0A21EE1}"/>
+    <hyperlink ref="H22" r:id="rId18" xr:uid="{834865A1-F184-4275-92B9-50D7586676F4}"/>
+    <hyperlink ref="H23" r:id="rId19" xr:uid="{1CB98BB8-55FC-48B7-8AFD-A442541FD20C}"/>
+    <hyperlink ref="H24" r:id="rId20" xr:uid="{61E9EF20-BF9E-498B-AA9D-B3D3D3805490}"/>
+    <hyperlink ref="H25" r:id="rId21" xr:uid="{8304FB56-2D2F-4429-B013-05499062E4B7}"/>
+    <hyperlink ref="H26" r:id="rId22" xr:uid="{399F4B86-142C-448A-8B9D-310755A67C4E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2114,11 +2159,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA4CCA6F-5860-423A-BE35-DCF970A6FC6C}">
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2139,48 +2184,48 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="J1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="M1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="N1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>190</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -2190,19 +2235,19 @@
         <v>pico-vga C1, C3, C5</v>
       </c>
       <c r="D2" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="E2" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="I2" s="1">
         <v>0.28999999999999998</v>
@@ -2215,38 +2260,38 @@
         <v>0.86999999999999988</v>
       </c>
       <c r="M2" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="N2" s="1">
         <f>SUM(K:K)</f>
-        <v>13.639999999999997</v>
+        <v>13.839999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C25" si="0">_xlfn.CONCAT($N$1, B3)</f>
+        <f t="shared" ref="C3:C26" si="0">_xlfn.CONCAT($N$1, B3)</f>
         <v>pico-vga C2, C4</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="E3" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="I3" s="1">
         <v>0.1</v>
@@ -2255,13 +2300,13 @@
         <v>2</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K51" si="1">I3*J3</f>
+        <f t="shared" ref="K3:K52" si="1">I3*J3</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -2271,16 +2316,16 @@
         <v>pico-vga D1</v>
       </c>
       <c r="D4" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="E4" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="I4" s="1">
         <v>0.19</v>
@@ -2295,7 +2340,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -2308,13 +2353,13 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="I5" s="1">
         <v>0.21</v>
@@ -2329,7 +2374,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
@@ -2342,13 +2387,13 @@
         <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="I6" s="1">
         <v>1.46</v>
@@ -2363,7 +2408,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
@@ -2373,16 +2418,16 @@
         <v>pico-vga J2</v>
       </c>
       <c r="D7" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="E7" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="I7" s="1">
         <v>1.2</v>
@@ -2397,26 +2442,26 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga J3, J4, J8, J9</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="I8" s="1">
         <v>0.48</v>
@@ -2431,17 +2476,17 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga J5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -2453,26 +2498,26 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga J6</v>
       </c>
       <c r="D10" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="E10" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="I10" s="1">
         <v>0.8</v>
@@ -2487,17 +2532,17 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga J7</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -2509,26 +2554,26 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga Q1</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="I12" s="1">
         <v>0.34</v>
@@ -2543,29 +2588,29 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>192</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R1, R12</v>
+        <v>pico-vga R1, R14</v>
       </c>
       <c r="D13" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="E13" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="I13" s="1">
         <v>0.1</v>
@@ -2580,29 +2625,29 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>107</v>
+        <v>193</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga R2, R6</v>
       </c>
       <c r="D14" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="E14" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="I14" s="1">
         <v>0.1</v>
@@ -2617,29 +2662,29 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>194</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga R3, R7</v>
       </c>
       <c r="D15" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="E15" t="s">
-        <v>180</v>
+        <v>154</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="I15" s="1">
         <v>0.1</v>
@@ -2654,29 +2699,29 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>109</v>
+        <v>195</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga R4, R8</v>
       </c>
       <c r="D16" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="E16" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="I16" s="1">
         <v>0.1</v>
@@ -2691,29 +2736,29 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>196</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga R5, R9</v>
       </c>
       <c r="D17" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="E17" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="I17" s="1">
         <v>0.1</v>
@@ -2728,66 +2773,66 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>197</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>180</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R10</v>
+        <v>pico-vga R10, R11</v>
       </c>
       <c r="D18" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="E18" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>133</v>
+        <v>181</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="I18" s="1">
         <v>0.1</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K18" s="1">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>198</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>182</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R11</v>
+        <v>pico-vga R12</v>
       </c>
       <c r="D19" t="s">
-        <v>191</v>
+        <v>150</v>
       </c>
       <c r="E19" t="s">
-        <v>192</v>
+        <v>151</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>193</v>
+        <v>152</v>
       </c>
       <c r="I19" s="1">
         <v>0.1</v>
@@ -2802,103 +2847,103 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>199</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>183</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R13, R17, R18, R22, R23</v>
+        <v>pico-vga R13</v>
       </c>
       <c r="D20" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="E20" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="I20" s="1">
         <v>0.1</v>
       </c>
       <c r="J20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K20" s="1">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>200</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R14, R19</v>
+        <v>pico-vga R15, R19, R20, R24, R25</v>
       </c>
       <c r="D21" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="E21" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>135</v>
+        <v>59</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="I21" s="1">
         <v>0.1</v>
       </c>
       <c r="J21">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K21" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>201</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R15, R20</v>
+        <v>pico-vga R16, R21</v>
       </c>
       <c r="D22" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="E22" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="I22" s="1">
         <v>0.1</v>
@@ -2913,29 +2958,29 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>202</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>185</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R16, R21</v>
+        <v>pico-vga R17, R22</v>
       </c>
       <c r="D23" t="s">
-        <v>188</v>
+        <v>141</v>
       </c>
       <c r="E23" t="s">
-        <v>189</v>
+        <v>142</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>190</v>
+        <v>143</v>
       </c>
       <c r="I23" s="1">
         <v>0.1</v>
@@ -2950,76 +2995,107 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>117</v>
+        <v>203</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>186</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga SW1</v>
+        <v>pico-vga R18, R23</v>
       </c>
       <c r="D24" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="E24" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>124</v>
+        <v>93</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="I24" s="1">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="J24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K24" s="1">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga U1</v>
+        <v>pico-vga SW1</v>
       </c>
       <c r="D25" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="E25" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="I25" s="1">
-        <v>4</v>
+        <v>0.15</v>
       </c>
       <c r="J25">
         <v>1</v>
       </c>
       <c r="K25" s="1">
         <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>pico-vga U1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I26" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J26">
+        <v>1</v>
+      </c>
       <c r="K26" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -3168,6 +3244,12 @@
     </row>
     <row r="51" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K51" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K52" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3189,14 +3271,14 @@
     <hyperlink ref="H15" r:id="rId12" xr:uid="{082DD5BC-6FD7-4E37-82D5-7429DFC70929}"/>
     <hyperlink ref="H16" r:id="rId13" xr:uid="{A6BB3CBA-1409-4B40-9526-00CA096EE12C}"/>
     <hyperlink ref="H17" r:id="rId14" xr:uid="{E5BA8CAD-41D4-4EBE-A9B6-A757FAAE7956}"/>
-    <hyperlink ref="H18" r:id="rId15" xr:uid="{92667990-6046-4061-A4CC-A42B6474DDC3}"/>
-    <hyperlink ref="H19" r:id="rId16" xr:uid="{21F8108C-9D28-434A-9355-4756E6529366}"/>
-    <hyperlink ref="H20" r:id="rId17" xr:uid="{CD94A188-E20E-470A-B31C-503D210C3E0F}"/>
-    <hyperlink ref="H21" r:id="rId18" xr:uid="{026CEBAD-F722-4781-B8FD-C5943F91AAF1}"/>
-    <hyperlink ref="H22" r:id="rId19" xr:uid="{035A57E6-C5E2-4340-BE4E-B2D2FD0BE4AE}"/>
-    <hyperlink ref="H23" r:id="rId20" xr:uid="{0EAEB1F1-4426-471A-ABBE-2E4BA652B2D7}"/>
-    <hyperlink ref="H24" r:id="rId21" xr:uid="{F2529482-D2C9-4889-81E1-9803E39972F3}"/>
-    <hyperlink ref="H25" r:id="rId22" xr:uid="{A024EAD0-F1A3-454C-AFA6-7BC8B85A951B}"/>
+    <hyperlink ref="H19" r:id="rId15" xr:uid="{92667990-6046-4061-A4CC-A42B6474DDC3}"/>
+    <hyperlink ref="H20" r:id="rId16" xr:uid="{21F8108C-9D28-434A-9355-4756E6529366}"/>
+    <hyperlink ref="H21" r:id="rId17" xr:uid="{CD94A188-E20E-470A-B31C-503D210C3E0F}"/>
+    <hyperlink ref="H22" r:id="rId18" xr:uid="{026CEBAD-F722-4781-B8FD-C5943F91AAF1}"/>
+    <hyperlink ref="H23" r:id="rId19" xr:uid="{035A57E6-C5E2-4340-BE4E-B2D2FD0BE4AE}"/>
+    <hyperlink ref="H24" r:id="rId20" xr:uid="{0EAEB1F1-4426-471A-ABBE-2E4BA652B2D7}"/>
+    <hyperlink ref="H25" r:id="rId21" xr:uid="{F2529482-D2C9-4889-81E1-9803E39972F3}"/>
+    <hyperlink ref="H26" r:id="rId22" xr:uid="{A024EAD0-F1A3-454C-AFA6-7BC8B85A951B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3204,11 +3286,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB529BA2-03A0-4F42-AB88-7E5D455824D2}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3373,19 +3453,19 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>174</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>175</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>176</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>177</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -3396,22 +3476,22 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
         <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -3422,16 +3502,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
         <v>12</v>
@@ -3445,22 +3525,22 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>178</v>
       </c>
       <c r="G10" t="s">
         <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>48</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -3471,16 +3551,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G11" t="s">
         <v>12</v>
@@ -3494,22 +3574,22 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G12" t="s">
         <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -3520,16 +3600,16 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G13" t="s">
         <v>12</v>
@@ -3543,16 +3623,16 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D14">
         <v>470</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G14" t="s">
         <v>12</v>
@@ -3566,16 +3646,16 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D15">
         <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G15" t="s">
         <v>12</v>
@@ -3589,16 +3669,16 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G16" t="s">
         <v>12</v>
@@ -3612,16 +3692,16 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G17" t="s">
         <v>12</v>
@@ -3632,19 +3712,19 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18">
-        <v>390</v>
+        <v>180</v>
+      </c>
+      <c r="D18" t="s">
+        <v>181</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G18" t="s">
         <v>12</v>
@@ -3658,16 +3738,16 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>182</v>
       </c>
       <c r="D19">
-        <v>47</v>
+        <v>390</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G19" t="s">
         <v>12</v>
@@ -3678,19 +3758,19 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" t="s">
-        <v>70</v>
+        <v>183</v>
+      </c>
+      <c r="D20">
+        <v>47</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G20" t="s">
         <v>12</v>
@@ -3701,19 +3781,19 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21">
-        <v>220</v>
+        <v>184</v>
+      </c>
+      <c r="D21" t="s">
+        <v>59</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F21" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G21" t="s">
         <v>12</v>
@@ -3727,16 +3807,16 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D22">
-        <v>100</v>
+        <v>220</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F22" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G22" t="s">
         <v>12</v>
@@ -3750,16 +3830,16 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" t="s">
-        <v>74</v>
+        <v>185</v>
+      </c>
+      <c r="D23">
+        <v>100</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G23" t="s">
         <v>12</v>
@@ -3770,19 +3850,19 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>186</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="F24" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="G24" t="s">
         <v>12</v>
@@ -3796,16 +3876,39 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="D25" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="E25" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="F25" t="s">
-        <v>81</v>
+        <v>65</v>
+      </c>
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Forgot I2C pullup resistors, updated Sch, PCB, and BOM"
Don't need the pullups, you can do it internally in software. No point adding them and making the BOM longer.

This reverts commit bd8d0dffae4885964e3fb42256447820ac871936.
</commit_message>
<xml_diff>
--- a/docs/BOM.xlsx
+++ b/docs/BOM.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\DATA\Projects\pico-vga\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8847281D-C444-473F-9E5D-F2863FF23E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F069ADD-8B6D-4E77-82E6-B5A1EED384D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{135CBA0D-5FA5-414C-B0B9-8FCA77DD5795}"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM_Custom" sheetId="5" r:id="rId1"/>
+    <sheet name="BOM_Custom" sheetId="3" r:id="rId1"/>
     <sheet name="BOM" sheetId="2" r:id="rId2"/>
     <sheet name="BOM_Export" sheetId="1" r:id="rId3"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="200">
   <si>
     <t>Item</t>
   </si>
@@ -130,6 +130,21 @@
     <t>J2</t>
   </si>
   <si>
+    <t>Micro_SD_Card</t>
+  </si>
+  <si>
+    <t>Connector:Micro_SD_Card</t>
+  </si>
+  <si>
+    <t>Connector_Card:microSD_HC_Hirose_DM3AT-SF-PEJM5</t>
+  </si>
+  <si>
+    <t>http://katalog.we-online.de/em/datasheet/693072010801.pdf</t>
+  </si>
+  <si>
+    <t>DM3AT-SF-PEJM5</t>
+  </si>
+  <si>
     <t>J3, J4, J8, J9</t>
   </si>
   <si>
@@ -166,6 +181,12 @@
     <t>Connector:AudioJack3</t>
   </si>
   <si>
+    <t>Connector_Audio:Jack_3.5mm_CUI_SJ1-3533NG_Horizontal</t>
+  </si>
+  <si>
+    <t>SJ1-3533NG</t>
+  </si>
+  <si>
     <t>J7</t>
   </si>
   <si>
@@ -190,6 +211,9 @@
     <t>Package_TO_SOT_SMD:SOT-23</t>
   </si>
   <si>
+    <t>R1, R12</t>
+  </si>
+  <si>
     <t>1K</t>
   </si>
   <si>
@@ -217,9 +241,24 @@
     <t>2.2K</t>
   </si>
   <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R13, R17, R18, R22, R23</t>
+  </si>
+  <si>
     <t>1M</t>
   </si>
   <si>
+    <t>R14, R19</t>
+  </si>
+  <si>
+    <t>R15, R20</t>
+  </si>
+  <si>
     <t>R16, R21</t>
   </si>
   <si>
@@ -283,9 +322,15 @@
     <t>Total Cost</t>
   </si>
   <si>
+    <t>47uF 0805 Cap</t>
+  </si>
+  <si>
     <t xml:space="preserve">pico-vga </t>
   </si>
   <si>
+    <t>100nF 0805 Cap</t>
+  </si>
+  <si>
     <t>Blue LED 0805</t>
   </si>
   <si>
@@ -313,6 +358,39 @@
     <t>PMOS 30V 3.8A</t>
   </si>
   <si>
+    <t>1k 0805 Res</t>
+  </si>
+  <si>
+    <t>470R 0805 Res</t>
+  </si>
+  <si>
+    <t>33R 0805 Res</t>
+  </si>
+  <si>
+    <t>1.2k 0805 Res</t>
+  </si>
+  <si>
+    <t>2.2k 0805 Res</t>
+  </si>
+  <si>
+    <t>390R 0805 Res</t>
+  </si>
+  <si>
+    <t>47R 0805 Res</t>
+  </si>
+  <si>
+    <t>1M 0805 Res</t>
+  </si>
+  <si>
+    <t>220R 0805 Res</t>
+  </si>
+  <si>
+    <t>100R 0805 Res</t>
+  </si>
+  <si>
+    <t>1.8k 0805 Res</t>
+  </si>
+  <si>
     <t>Reset Button</t>
   </si>
   <si>
@@ -560,96 +638,6 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21B104KBCNNNC/3886661</t>
-  </si>
-  <si>
-    <t>Micro_SD_Card_Det</t>
-  </si>
-  <si>
-    <t>Connector:Micro_SD_Card_Det</t>
-  </si>
-  <si>
-    <t>pico-vga:MEM2061-01-188-00-A_GCT</t>
-  </si>
-  <si>
-    <t>https://www.hirose.com/product/en/download_file/key_name/DM3/category/Catalog/doc_file_id/49662/?file_category_id=4&amp;item_id=195&amp;is_series=1</t>
-  </si>
-  <si>
-    <t>pico-vga:STX-3000_KYC</t>
-  </si>
-  <si>
-    <t>R1, R14</t>
-  </si>
-  <si>
-    <t>R10, R11</t>
-  </si>
-  <si>
-    <t>4.7k</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>R15, R19, R20, R24, R25</t>
-  </si>
-  <si>
-    <t>R17, R22</t>
-  </si>
-  <si>
-    <t>R18, R23</t>
-  </si>
-  <si>
-    <t>ERJ-6ENF4701V</t>
-  </si>
-  <si>
-    <t>P4.70KCCT-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-6ENF4701V/954352?s=N4IgjCBcoExaBjKAzAhgGwM4FMA0IB7KAbXAAYAOAdgE4QBdfABwBcoQBlFgJwEsA7AOYgAvvgDM8EEkhoseQiXBhxERiFbsufIaPxgAbFJlyc%2BIpFLia4mHXWbInHgOFjwNCnWjSUGM4qWIGQM7jCUAKzGfvLmSgAsAHRUAAQA1gDyABYAtpgMzGxOAKr8vCwZyACy2KiYAK7c2HogALRwPjI89QoWpFH07q1GnVDdvUqSg-it3ohj3D1xQWpDEKOy-hMrIYNhSk2YvJgsBNyhQA</t>
-  </si>
-  <si>
-    <t>47uF 0805 Cap (5V or more)</t>
-  </si>
-  <si>
-    <t>100nF 0805 Cap (5V or more)</t>
-  </si>
-  <si>
-    <t>1k 0805 Res 1%</t>
-  </si>
-  <si>
-    <t>470R 0805 Res 1%</t>
-  </si>
-  <si>
-    <t>33R 0805 Res 1%</t>
-  </si>
-  <si>
-    <t>1.2k 0805 Res 1%</t>
-  </si>
-  <si>
-    <t>2.2k 0805 Res 1%</t>
-  </si>
-  <si>
-    <t>4.7k 0805 Res 1%</t>
-  </si>
-  <si>
-    <t>390R 0805 Res 1%</t>
-  </si>
-  <si>
-    <t>47R 0805 Res 1%</t>
-  </si>
-  <si>
-    <t>1M 0805 Res 1%</t>
-  </si>
-  <si>
-    <t>220R 0805 Res 1%</t>
-  </si>
-  <si>
-    <t>100R 0805 Res 1%</t>
-  </si>
-  <si>
-    <t>1.8k 0805 Res 1%</t>
   </si>
 </sst>
 </file>
@@ -734,6 +722,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1032,8 +1024,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCE2567-DB3F-4561-9ED3-12DD0FC8DD03}">
-  <dimension ref="A1:N52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41676850-015E-4523-B008-90A3DF7CB11C}">
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1058,48 +1050,48 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="J1" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="M1" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="N1" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1109,19 +1101,19 @@
         <v>pico-vga C1, C3, C5</v>
       </c>
       <c r="D2" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="I2" s="1">
         <v>0.28999999999999998</v>
@@ -1134,38 +1126,38 @@
         <v>0.86999999999999988</v>
       </c>
       <c r="M2" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="N2" s="1">
         <f>SUM(K:K)</f>
-        <v>13.839999999999996</v>
+        <v>13.639999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C26" si="0">_xlfn.CONCAT($N$1, B3)</f>
+        <f t="shared" ref="C3:C25" si="0">_xlfn.CONCAT($N$1, B3)</f>
         <v>pico-vga C2, C4</v>
       </c>
       <c r="D3" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="E3" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="I3" s="1">
         <v>0.1</v>
@@ -1174,13 +1166,13 @@
         <v>2</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K52" si="1">I3*J3</f>
+        <f t="shared" ref="K3:K51" si="1">I3*J3</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -1190,16 +1182,16 @@
         <v>pico-vga D1</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="E4" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="I4" s="1">
         <v>0.19</v>
@@ -1214,7 +1206,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -1227,13 +1219,13 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="I5" s="1">
         <v>0.21</v>
@@ -1248,7 +1240,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
@@ -1261,13 +1253,13 @@
         <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="I6" s="1">
         <v>1.46</v>
@@ -1282,7 +1274,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
@@ -1292,16 +1284,16 @@
         <v>pico-vga J2</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="E7" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="I7" s="1">
         <v>1.2</v>
@@ -1316,26 +1308,26 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga J3, J4, J8, J9</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="I8" s="1">
         <v>0.48</v>
@@ -1350,17 +1342,17 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga J5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -1372,26 +1364,26 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga J6</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="I10" s="1">
         <v>0.8</v>
@@ -1406,17 +1398,17 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga J7</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1428,26 +1420,26 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga Q1</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="I12" s="1">
         <v>0.34</v>
@@ -1462,29 +1454,29 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>106</v>
       </c>
       <c r="B13" t="s">
-        <v>179</v>
+        <v>57</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R1, R14</v>
+        <v>pico-vga R1, R12</v>
       </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
       <c r="E13" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="I13" s="1">
         <v>0.1</v>
@@ -1499,29 +1491,29 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>107</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga R2, R6</v>
       </c>
       <c r="D14" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="I14" s="1">
         <v>0.1</v>
@@ -1536,29 +1528,29 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>194</v>
+        <v>108</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga R3, R7</v>
       </c>
       <c r="D15" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="E15" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="I15" s="1">
         <v>0.1</v>
@@ -1573,29 +1565,29 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>109</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga R4, R8</v>
       </c>
       <c r="D16" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="E16" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="I16" s="1">
         <v>0.1</v>
@@ -1610,29 +1602,29 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>110</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga R5, R9</v>
       </c>
       <c r="D17" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
       <c r="E17" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>158</v>
+        <v>184</v>
       </c>
       <c r="I17" s="1">
         <v>0.1</v>
@@ -1647,66 +1639,66 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>197</v>
+        <v>111</v>
       </c>
       <c r="B18" t="s">
-        <v>180</v>
+        <v>67</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R10, R11</v>
+        <v>pico-vga R10</v>
       </c>
       <c r="D18" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="E18" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>181</v>
+        <v>133</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="I18" s="1">
         <v>0.1</v>
       </c>
       <c r="J18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K18" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>198</v>
+        <v>112</v>
       </c>
       <c r="B19" t="s">
-        <v>182</v>
+        <v>68</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R12</v>
+        <v>pico-vga R11</v>
       </c>
       <c r="D19" t="s">
-        <v>150</v>
+        <v>191</v>
       </c>
       <c r="E19" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>152</v>
+        <v>193</v>
       </c>
       <c r="I19" s="1">
         <v>0.1</v>
@@ -1721,103 +1713,103 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>199</v>
+        <v>113</v>
       </c>
       <c r="B20" t="s">
-        <v>183</v>
+        <v>69</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R13</v>
+        <v>pico-vga R13, R17, R18, R22, R23</v>
       </c>
       <c r="D20" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="E20" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="I20" s="1">
         <v>0.1</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K20" s="1">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>200</v>
+        <v>114</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>71</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R15, R19, R20, R24, R25</v>
+        <v>pico-vga R14, R19</v>
       </c>
       <c r="D21" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="E21" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="I21" s="1">
         <v>0.1</v>
       </c>
       <c r="J21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K21" s="1">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>201</v>
+        <v>115</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R16, R21</v>
+        <v>pico-vga R15, R20</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="E22" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="I22" s="1">
         <v>0.1</v>
@@ -1832,29 +1824,29 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>202</v>
+        <v>116</v>
       </c>
       <c r="B23" t="s">
-        <v>185</v>
+        <v>73</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R17, R22</v>
+        <v>pico-vga R16, R21</v>
       </c>
       <c r="D23" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="E23" t="s">
-        <v>142</v>
+        <v>189</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>143</v>
+        <v>190</v>
       </c>
       <c r="I23" s="1">
         <v>0.1</v>
@@ -1869,107 +1861,76 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>203</v>
+        <v>117</v>
       </c>
       <c r="B24" t="s">
-        <v>186</v>
+        <v>75</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R18, R23</v>
+        <v>pico-vga SW1</v>
       </c>
       <c r="D24" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="E24" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="I24" s="1">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="J24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K24" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga SW1</v>
+        <v>pico-vga U1</v>
       </c>
       <c r="D25" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="E25" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="I25" s="1">
-        <v>0.15</v>
+        <v>4</v>
       </c>
       <c r="J25">
         <v>1</v>
       </c>
       <c r="K25" s="1">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>92</v>
-      </c>
-      <c r="B26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" t="str">
-        <f t="shared" si="0"/>
-        <v>pico-vga U1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>112</v>
-      </c>
-      <c r="E26" t="s">
-        <v>113</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="I26" s="1">
-        <v>4</v>
-      </c>
-      <c r="J26">
-        <v>1</v>
-      </c>
       <c r="K26" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -2122,36 +2083,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K52" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{C47512F7-0DAA-4BE6-BFA1-26DEE74CB3CA}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{BC6569AC-BC35-4D24-904A-6ABDA5EDC7CE}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{8776341B-3204-4BB0-8D0E-0F3D826EEAA5}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{7C44B87C-08D8-4941-90D3-24044D980DCC}"/>
-    <hyperlink ref="H6" r:id="rId5" xr:uid="{1C21CAEB-46F7-4AFB-97D8-FDE88EE1E357}"/>
-    <hyperlink ref="H7" r:id="rId6" xr:uid="{7B497EAA-CA7E-4F20-9B1B-CB46AF8EF7AA}"/>
-    <hyperlink ref="H8" r:id="rId7" xr:uid="{BED54906-8ACB-4F14-83C2-2222E2F1601F}"/>
-    <hyperlink ref="H10" r:id="rId8" xr:uid="{61F094BB-133C-4849-AA5E-A64E986F6577}"/>
-    <hyperlink ref="H12" r:id="rId9" xr:uid="{5874167A-891D-4902-910D-BEB10AC847DA}"/>
-    <hyperlink ref="H13" r:id="rId10" display="https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-6ENF1001V/111281?s=N4IgjCBcoExaBjKAzAhgGwM4FMA0IB7KAbXAAYAOAdgE4QBdfABwBcoQBlFgJwEsA7AOYgAvvgDM8EEkhoseQiXBhxERiFbsufIaPxgAbFJlyc%2BIpFLia4mHXWbInHgOFjwNCnWjSUGM4qWIGQM7jCUAKzGfvLmSmAABADWAPIAFgC2mAzMbE4Aqvy8LCnIALLYqJgArtzYeiAAtHA%2BMjzVChakUfTujUatUO2dSpK9%2BI3eiEPcHXFBan0Qg7L%2BIwshvWFKdZi8mCwE3KFAA" xr:uid="{843498AC-23AF-4C7C-8E69-6933C2F6B689}"/>
-    <hyperlink ref="H14" r:id="rId11" display="https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-6ENF4700V/1746508?s=N4IgjCBcoExaBjKAzAhgGwM4FMA0IB7KAbXAAYAOAdgE4QBdfABwBcoQBlFgJwEsA7AOYgAvvgDM8EEkhoseQiXBhxERiFbsufIaPxgAbFJlyc%2BIpFLia4mHXWbInHgOFjwNCnWjSUGM4qWIGQM7jCUAKzGfvLmSgAsVGQABADyABYAtpgMzGxOAKr8vCypyACy2KiYAK7c2HogALRwPjI8NQoWpFH07k1GbVAdXUqSffhN3ojD3J1xQWr9EEOy-qOLIX1hSvWYvJgsBNyhQA" xr:uid="{FDC50D01-9324-4EBE-9031-1BB648303976}"/>
-    <hyperlink ref="H15" r:id="rId12" xr:uid="{71D2F41C-2893-424A-9F76-A0C70CEA3650}"/>
-    <hyperlink ref="H16" r:id="rId13" xr:uid="{83E26751-A6AF-41B3-8035-689D68DBBED3}"/>
-    <hyperlink ref="H17" r:id="rId14" xr:uid="{97E5C901-985C-41ED-80E5-9AA69D90C7B2}"/>
-    <hyperlink ref="H19" r:id="rId15" xr:uid="{EC43C74C-3F6A-41D7-9417-ACA2B8768492}"/>
-    <hyperlink ref="H20" r:id="rId16" xr:uid="{31CAC340-61BC-4528-9984-0AE84D3560AF}"/>
-    <hyperlink ref="H21" r:id="rId17" xr:uid="{6C616E04-52D4-42F5-BA64-8BACA0A21EE1}"/>
-    <hyperlink ref="H22" r:id="rId18" xr:uid="{834865A1-F184-4275-92B9-50D7586676F4}"/>
-    <hyperlink ref="H23" r:id="rId19" xr:uid="{1CB98BB8-55FC-48B7-8AFD-A442541FD20C}"/>
-    <hyperlink ref="H24" r:id="rId20" xr:uid="{61E9EF20-BF9E-498B-AA9D-B3D3D3805490}"/>
-    <hyperlink ref="H25" r:id="rId21" xr:uid="{8304FB56-2D2F-4429-B013-05499062E4B7}"/>
-    <hyperlink ref="H26" r:id="rId22" xr:uid="{399F4B86-142C-448A-8B9D-310755A67C4E}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{C3943670-D334-4FAC-881A-C084D9B4E51D}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{8453B33C-E27C-4A6E-9F24-76167FFE0D5A}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{1F45F393-7E29-4563-A41D-32FCA93B4E9E}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{E8AB2F55-D124-4C88-BE93-7754876E1F99}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{86E8A67A-7938-4329-AE54-7FA7B8E27164}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{F6F87F88-AF48-4CFC-BE3F-215EA6808536}"/>
+    <hyperlink ref="H8" r:id="rId7" xr:uid="{5C139857-F57C-47E5-A665-B00AE15616F8}"/>
+    <hyperlink ref="H10" r:id="rId8" xr:uid="{F6887023-ECBA-4F1A-879C-0915165C147A}"/>
+    <hyperlink ref="H12" r:id="rId9" xr:uid="{E23B089E-DC5A-446B-A089-3D0D291CB77B}"/>
+    <hyperlink ref="H13" r:id="rId10" display="https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-6ENF1001V/111281?s=N4IgjCBcoExaBjKAzAhgGwM4FMA0IB7KAbXAAYAOAdgE4QBdfABwBcoQBlFgJwEsA7AOYgAvvgDM8EEkhoseQiXBhxERiFbsufIaPxgAbFJlyc%2BIpFLia4mHXWbInHgOFjwNCnWjSUGM4qWIGQM7jCUAKzGfvLmSmAABADWAPIAFgC2mAzMbE4Aqvy8LCnIALLYqJgArtzYeiAAtHA%2BMjzVChakUfTujUatUO2dSpK9%2BI3eiEPcHXFBan0Qg7L%2BIwshvWFKdZi8mCwE3KFAA" xr:uid="{A88E5C24-E592-4AC2-8381-4ACA653CD105}"/>
+    <hyperlink ref="H14" r:id="rId11" display="https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-6ENF4700V/1746508?s=N4IgjCBcoExaBjKAzAhgGwM4FMA0IB7KAbXAAYAOAdgE4QBdfABwBcoQBlFgJwEsA7AOYgAvvgDM8EEkhoseQiXBhxERiFbsufIaPxgAbFJlyc%2BIpFLia4mHXWbInHgOFjwNCnWjSUGM4qWIGQM7jCUAKzGfvLmSgAsVGQABADyABYAtpgMzGxOAKr8vCypyACy2KiYAK7c2HogALRwPjI8NQoWpFH07k1GbVAdXUqSffhN3ojD3J1xQWr9EEOy-qOLIX1hSvWYvJgsBNyhQA" xr:uid="{20CAD594-E534-4122-9C9E-5CBB98259CB8}"/>
+    <hyperlink ref="H15" r:id="rId12" xr:uid="{D9C0AA91-F664-471A-83D0-99DC5DE48B04}"/>
+    <hyperlink ref="H16" r:id="rId13" xr:uid="{23053BEB-EE99-4ABB-B9B0-7CED281F5C88}"/>
+    <hyperlink ref="H17" r:id="rId14" xr:uid="{E34D31C8-B691-48B5-894A-976DD7FA5A9A}"/>
+    <hyperlink ref="H18" r:id="rId15" xr:uid="{DC30CFD1-5C16-4F7A-B6B2-7B063165F47C}"/>
+    <hyperlink ref="H19" r:id="rId16" xr:uid="{64D4C0A7-868D-4DF8-AA3D-CE0709999D55}"/>
+    <hyperlink ref="H20" r:id="rId17" xr:uid="{829A5152-1413-4ED1-AD65-2ACE37C987CE}"/>
+    <hyperlink ref="H21" r:id="rId18" xr:uid="{DDB86A52-C5B3-46D5-8ABC-099C6554353C}"/>
+    <hyperlink ref="H22" r:id="rId19" xr:uid="{6FCAB29C-A9A8-445E-965A-3B77996ACB2B}"/>
+    <hyperlink ref="H23" r:id="rId20" xr:uid="{3971B7D7-1F62-4C22-8071-CF13C66BFDEA}"/>
+    <hyperlink ref="H24" r:id="rId21" xr:uid="{A8E5EF7B-3BB3-4864-B86C-B008FB819D0A}"/>
+    <hyperlink ref="H25" r:id="rId22" xr:uid="{53CB6B44-1923-4935-BF28-705CDC91EF58}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2159,11 +2114,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA4CCA6F-5860-423A-BE35-DCF970A6FC6C}">
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2184,48 +2139,48 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="J1" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="M1" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="N1" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -2235,19 +2190,19 @@
         <v>pico-vga C1, C3, C5</v>
       </c>
       <c r="D2" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="I2" s="1">
         <v>0.28999999999999998</v>
@@ -2260,38 +2215,38 @@
         <v>0.86999999999999988</v>
       </c>
       <c r="M2" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="N2" s="1">
         <f>SUM(K:K)</f>
-        <v>13.839999999999996</v>
+        <v>13.639999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C26" si="0">_xlfn.CONCAT($N$1, B3)</f>
+        <f t="shared" ref="C3:C25" si="0">_xlfn.CONCAT($N$1, B3)</f>
         <v>pico-vga C2, C4</v>
       </c>
       <c r="D3" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="E3" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="I3" s="1">
         <v>0.1</v>
@@ -2300,13 +2255,13 @@
         <v>2</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K52" si="1">I3*J3</f>
+        <f t="shared" ref="K3:K51" si="1">I3*J3</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -2316,16 +2271,16 @@
         <v>pico-vga D1</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="E4" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="I4" s="1">
         <v>0.19</v>
@@ -2340,7 +2295,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -2353,13 +2308,13 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="I5" s="1">
         <v>0.21</v>
@@ -2374,7 +2329,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
@@ -2387,13 +2342,13 @@
         <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="I6" s="1">
         <v>1.46</v>
@@ -2408,7 +2363,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
@@ -2418,16 +2373,16 @@
         <v>pico-vga J2</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="E7" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="I7" s="1">
         <v>1.2</v>
@@ -2442,26 +2397,26 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga J3, J4, J8, J9</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="I8" s="1">
         <v>0.48</v>
@@ -2476,17 +2431,17 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga J5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -2498,26 +2453,26 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga J6</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="I10" s="1">
         <v>0.8</v>
@@ -2532,17 +2487,17 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga J7</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -2554,26 +2509,26 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga Q1</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="I12" s="1">
         <v>0.34</v>
@@ -2588,29 +2543,29 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>106</v>
       </c>
       <c r="B13" t="s">
-        <v>179</v>
+        <v>57</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R1, R14</v>
+        <v>pico-vga R1, R12</v>
       </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
       <c r="E13" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="I13" s="1">
         <v>0.1</v>
@@ -2625,29 +2580,29 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>107</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga R2, R6</v>
       </c>
       <c r="D14" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="I14" s="1">
         <v>0.1</v>
@@ -2662,29 +2617,29 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>194</v>
+        <v>108</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga R3, R7</v>
       </c>
       <c r="D15" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="E15" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="I15" s="1">
         <v>0.1</v>
@@ -2699,29 +2654,29 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>109</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga R4, R8</v>
       </c>
       <c r="D16" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="E16" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="I16" s="1">
         <v>0.1</v>
@@ -2736,29 +2691,29 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>110</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>pico-vga R5, R9</v>
       </c>
       <c r="D17" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
       <c r="E17" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>158</v>
+        <v>184</v>
       </c>
       <c r="I17" s="1">
         <v>0.1</v>
@@ -2773,66 +2728,66 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>197</v>
+        <v>111</v>
       </c>
       <c r="B18" t="s">
-        <v>180</v>
+        <v>67</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R10, R11</v>
+        <v>pico-vga R10</v>
       </c>
       <c r="D18" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="E18" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>181</v>
+        <v>133</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="I18" s="1">
         <v>0.1</v>
       </c>
       <c r="J18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K18" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>198</v>
+        <v>112</v>
       </c>
       <c r="B19" t="s">
-        <v>182</v>
+        <v>68</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R12</v>
+        <v>pico-vga R11</v>
       </c>
       <c r="D19" t="s">
-        <v>150</v>
+        <v>191</v>
       </c>
       <c r="E19" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>152</v>
+        <v>193</v>
       </c>
       <c r="I19" s="1">
         <v>0.1</v>
@@ -2847,103 +2802,103 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>199</v>
+        <v>113</v>
       </c>
       <c r="B20" t="s">
-        <v>183</v>
+        <v>69</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R13</v>
+        <v>pico-vga R13, R17, R18, R22, R23</v>
       </c>
       <c r="D20" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="E20" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="I20" s="1">
         <v>0.1</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K20" s="1">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>200</v>
+        <v>114</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>71</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R15, R19, R20, R24, R25</v>
+        <v>pico-vga R14, R19</v>
       </c>
       <c r="D21" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="E21" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="I21" s="1">
         <v>0.1</v>
       </c>
       <c r="J21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K21" s="1">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>201</v>
+        <v>115</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R16, R21</v>
+        <v>pico-vga R15, R20</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="E22" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="I22" s="1">
         <v>0.1</v>
@@ -2958,29 +2913,29 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>202</v>
+        <v>116</v>
       </c>
       <c r="B23" t="s">
-        <v>185</v>
+        <v>73</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R17, R22</v>
+        <v>pico-vga R16, R21</v>
       </c>
       <c r="D23" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="E23" t="s">
-        <v>142</v>
+        <v>189</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>143</v>
+        <v>190</v>
       </c>
       <c r="I23" s="1">
         <v>0.1</v>
@@ -2995,107 +2950,76 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>203</v>
+        <v>117</v>
       </c>
       <c r="B24" t="s">
-        <v>186</v>
+        <v>75</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga R18, R23</v>
+        <v>pico-vga SW1</v>
       </c>
       <c r="D24" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="E24" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="I24" s="1">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="J24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K24" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>pico-vga SW1</v>
+        <v>pico-vga U1</v>
       </c>
       <c r="D25" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="E25" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="I25" s="1">
-        <v>0.15</v>
+        <v>4</v>
       </c>
       <c r="J25">
         <v>1</v>
       </c>
       <c r="K25" s="1">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>92</v>
-      </c>
-      <c r="B26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" t="str">
-        <f t="shared" si="0"/>
-        <v>pico-vga U1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>112</v>
-      </c>
-      <c r="E26" t="s">
-        <v>113</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="I26" s="1">
-        <v>4</v>
-      </c>
-      <c r="J26">
-        <v>1</v>
-      </c>
       <c r="K26" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -3244,12 +3168,6 @@
     </row>
     <row r="51" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K51" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="11:11" x14ac:dyDescent="0.35">
-      <c r="K52" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3271,14 +3189,14 @@
     <hyperlink ref="H15" r:id="rId12" xr:uid="{082DD5BC-6FD7-4E37-82D5-7429DFC70929}"/>
     <hyperlink ref="H16" r:id="rId13" xr:uid="{A6BB3CBA-1409-4B40-9526-00CA096EE12C}"/>
     <hyperlink ref="H17" r:id="rId14" xr:uid="{E5BA8CAD-41D4-4EBE-A9B6-A757FAAE7956}"/>
-    <hyperlink ref="H19" r:id="rId15" xr:uid="{92667990-6046-4061-A4CC-A42B6474DDC3}"/>
-    <hyperlink ref="H20" r:id="rId16" xr:uid="{21F8108C-9D28-434A-9355-4756E6529366}"/>
-    <hyperlink ref="H21" r:id="rId17" xr:uid="{CD94A188-E20E-470A-B31C-503D210C3E0F}"/>
-    <hyperlink ref="H22" r:id="rId18" xr:uid="{026CEBAD-F722-4781-B8FD-C5943F91AAF1}"/>
-    <hyperlink ref="H23" r:id="rId19" xr:uid="{035A57E6-C5E2-4340-BE4E-B2D2FD0BE4AE}"/>
-    <hyperlink ref="H24" r:id="rId20" xr:uid="{0EAEB1F1-4426-471A-ABBE-2E4BA652B2D7}"/>
-    <hyperlink ref="H25" r:id="rId21" xr:uid="{F2529482-D2C9-4889-81E1-9803E39972F3}"/>
-    <hyperlink ref="H26" r:id="rId22" xr:uid="{A024EAD0-F1A3-454C-AFA6-7BC8B85A951B}"/>
+    <hyperlink ref="H18" r:id="rId15" xr:uid="{92667990-6046-4061-A4CC-A42B6474DDC3}"/>
+    <hyperlink ref="H19" r:id="rId16" xr:uid="{21F8108C-9D28-434A-9355-4756E6529366}"/>
+    <hyperlink ref="H20" r:id="rId17" xr:uid="{CD94A188-E20E-470A-B31C-503D210C3E0F}"/>
+    <hyperlink ref="H21" r:id="rId18" xr:uid="{026CEBAD-F722-4781-B8FD-C5943F91AAF1}"/>
+    <hyperlink ref="H22" r:id="rId19" xr:uid="{035A57E6-C5E2-4340-BE4E-B2D2FD0BE4AE}"/>
+    <hyperlink ref="H23" r:id="rId20" xr:uid="{0EAEB1F1-4426-471A-ABBE-2E4BA652B2D7}"/>
+    <hyperlink ref="H24" r:id="rId21" xr:uid="{F2529482-D2C9-4889-81E1-9803E39972F3}"/>
+    <hyperlink ref="H25" r:id="rId22" xr:uid="{A024EAD0-F1A3-454C-AFA6-7BC8B85A951B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3286,9 +3204,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB529BA2-03A0-4F42-AB88-7E5D455824D2}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3453,19 +3373,19 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>174</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>175</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
-        <v>176</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>177</v>
+        <v>33</v>
       </c>
       <c r="H7" t="s">
-        <v>129</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -3476,22 +3396,22 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G8" t="s">
         <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -3502,16 +3422,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G9" t="s">
         <v>12</v>
@@ -3525,22 +3445,22 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F10" t="s">
-        <v>178</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
         <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>132</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -3551,16 +3471,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="G11" t="s">
         <v>12</v>
@@ -3574,22 +3494,22 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G12" t="s">
         <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -3600,16 +3520,16 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>179</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
         <v>12</v>
@@ -3623,16 +3543,16 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D14">
         <v>470</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G14" t="s">
         <v>12</v>
@@ -3646,16 +3566,16 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D15">
         <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F15" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G15" t="s">
         <v>12</v>
@@ -3669,16 +3589,16 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G16" t="s">
         <v>12</v>
@@ -3692,16 +3612,16 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G17" t="s">
         <v>12</v>
@@ -3712,19 +3632,19 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>180</v>
-      </c>
-      <c r="D18" t="s">
-        <v>181</v>
+        <v>67</v>
+      </c>
+      <c r="D18">
+        <v>390</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G18" t="s">
         <v>12</v>
@@ -3738,16 +3658,16 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>182</v>
+        <v>68</v>
       </c>
       <c r="D19">
-        <v>390</v>
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G19" t="s">
         <v>12</v>
@@ -3758,19 +3678,19 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D20">
-        <v>47</v>
+        <v>69</v>
+      </c>
+      <c r="D20" t="s">
+        <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F20" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G20" t="s">
         <v>12</v>
@@ -3781,19 +3701,19 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>184</v>
-      </c>
-      <c r="D21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21">
+        <v>220</v>
+      </c>
+      <c r="E21" t="s">
         <v>59</v>
       </c>
-      <c r="E21" t="s">
-        <v>51</v>
-      </c>
       <c r="F21" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G21" t="s">
         <v>12</v>
@@ -3807,16 +3727,16 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22">
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" t="s">
         <v>60</v>
-      </c>
-      <c r="D22">
-        <v>220</v>
-      </c>
-      <c r="E22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22" t="s">
-        <v>52</v>
       </c>
       <c r="G22" t="s">
         <v>12</v>
@@ -3830,16 +3750,16 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>185</v>
-      </c>
-      <c r="D23">
-        <v>100</v>
+        <v>73</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
       </c>
       <c r="E23" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F23" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G23" t="s">
         <v>12</v>
@@ -3850,19 +3770,19 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>186</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="E24" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="F24" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="G24" t="s">
         <v>12</v>
@@ -3876,39 +3796,16 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="F25" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" t="s">
-        <v>68</v>
-      </c>
-      <c r="F26" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>